<commit_message>
Update planning status, update themes UIUI
</commit_message>
<xml_diff>
--- a/docs/planning/planning.xlsx
+++ b/docs/planning/planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungp\movie\Final Project\docs\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungp\movie\docs\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEDEF12-ED18-429E-9BCE-2C0589B0A0B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A127E21-4B65-416A-83AA-6A613D43D304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="1" xr2:uid="{C19F09B8-63BC-4CE7-BFBE-7F2585E3E38B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
   <si>
     <t>#</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>On Progress</t>
-  </si>
-  <si>
-    <t>15/3/2025</t>
   </si>
   <si>
     <t>16/3/2025</t>
@@ -432,53 +429,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,7 +1000,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
@@ -1053,10 +1050,10 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="31">
+      <c r="A2" s="25">
         <v>0</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="25">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1081,8 +1078,8 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1105,8 +1102,8 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1119,18 +1116,18 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="J4" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1143,18 +1140,18 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="J5" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1167,142 +1164,142 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="16" t="s">
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="28">
+        <v>1</v>
+      </c>
+      <c r="B8" s="28">
+        <v>2</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="34">
-        <v>1</v>
-      </c>
-      <c r="B8" s="34">
-        <v>2</v>
-      </c>
-      <c r="C8" s="35" t="s">
+      <c r="D8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>44</v>
+      <c r="E8" s="35" t="s">
+        <v>43</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="36"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="38"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="36"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>42</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="36"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="24"/>
-      <c r="E11" s="40"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="46.3">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="37"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="31">
+      <c r="A14" s="25">
         <v>2</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="25">
         <v>3</v>
       </c>
-      <c r="C14" s="35" t="s">
-        <v>47</v>
+      <c r="C14" s="32" t="s">
+        <v>46</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>43</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -1313,179 +1310,169 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="36"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="24"/>
-      <c r="E15" s="27"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="36"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>42</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="36"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="24"/>
-      <c r="E17" s="27"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="46.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="37"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10" ht="14.15" customHeight="1">
-      <c r="A20" s="34">
+      <c r="A20" s="28">
         <v>3</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="28">
         <v>4</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>43</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="24"/>
-      <c r="E21" s="27"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.15" customHeight="1">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>42</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="27"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="46.3">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
@@ -1502,6 +1489,16 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Update planning, themes, SRS V1.1
</commit_message>
<xml_diff>
--- a/docs/planning/planning.xlsx
+++ b/docs/planning/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungp\movie\docs\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A127E21-4B65-416A-83AA-6A613D43D304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F845FC3E-AAED-408B-BC1D-0475FC0409A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="1" xr2:uid="{C19F09B8-63BC-4CE7-BFBE-7F2585E3E38B}"/>
   </bookViews>
@@ -16,26 +16,17 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>#</t>
   </si>
@@ -429,6 +420,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -441,15 +441,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -463,6 +454,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -470,12 +467,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,19 +808,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="19.4609375" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="27.35546875" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="16.35546875" customWidth="1"/>
-    <col min="8" max="8" width="15.640625" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.3828125" customWidth="1"/>
+    <col min="5" max="5" width="16.84375" customWidth="1"/>
+    <col min="6" max="6" width="17.4609375" customWidth="1"/>
+    <col min="7" max="7" width="16.3828125" customWidth="1"/>
+    <col min="8" max="8" width="15.61328125" customWidth="1"/>
+    <col min="9" max="9" width="20.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.45">
+    <row r="1" spans="1:9" ht="15.9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -858,7 +849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="70.75">
+    <row r="2" spans="1:9" ht="72.900000000000006">
       <c r="A2" s="22">
         <v>0</v>
       </c>
@@ -881,7 +872,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="42.45">
+    <row r="3" spans="1:9" ht="43.75">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="6" t="s">
@@ -900,7 +891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="70.75">
+    <row r="4" spans="1:9" ht="58.3">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="6" t="s">
@@ -930,7 +921,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="56.6">
+    <row r="6" spans="1:9" ht="58.3">
       <c r="A6" s="22">
         <v>1</v>
       </c>
@@ -953,7 +944,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="42.45">
+    <row r="7" spans="1:9" ht="43.75">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="6" t="s">
@@ -999,22 +990,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462C93F8-120E-4632-ABB3-2BBE6FCADDF9}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.78515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.35546875" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.92578125" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.84375" customWidth="1"/>
+    <col min="2" max="2" width="14.84375" customWidth="1"/>
+    <col min="3" max="3" width="33.765625" customWidth="1"/>
+    <col min="4" max="4" width="18.69140625" customWidth="1"/>
+    <col min="5" max="5" width="25.3046875" customWidth="1"/>
+    <col min="6" max="6" width="10.3828125" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" customWidth="1"/>
+    <col min="8" max="8" width="13.921875" customWidth="1"/>
+    <col min="9" max="9" width="12.53515625" customWidth="1"/>
+    <col min="10" max="10" width="16.84375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1050,10 +1041,10 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="25">
+      <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="28">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1078,8 +1069,8 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1102,8 +1093,8 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1126,8 +1117,8 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1150,8 +1141,8 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1174,22 +1165,22 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="29"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="28">
+      <c r="A8" s="31">
         <v>1</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="31">
         <v>2</v>
       </c>
       <c r="C8" s="32" t="s">
@@ -1210,11 +1201,11 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="33"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="36"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -1224,13 +1215,13 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="33"/>
       <c r="D10" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="39" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="15"/>
@@ -1242,11 +1233,11 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="33"/>
       <c r="D11" s="24"/>
-      <c r="E11" s="38"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -1256,8 +1247,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="46.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="34"/>
       <c r="D12" s="15" t="s">
         <v>41</v>
@@ -1274,205 +1265,171 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="25">
+      <c r="A14" s="28">
         <v>2</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="28">
         <v>3</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>43</v>
-      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="17"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="16" t="s">
-        <v>33</v>
-      </c>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="33"/>
       <c r="D15" s="24"/>
-      <c r="E15" s="39"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="33"/>
-      <c r="D16" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>42</v>
-      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="33"/>
       <c r="D17" s="24"/>
-      <c r="E17" s="39"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="46.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.45">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="34"/>
-      <c r="D18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>44</v>
-      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
-      <c r="J18" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="J18" s="16"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="14.15" customHeight="1">
-      <c r="A20" s="28">
+      <c r="A20" s="31">
         <v>3</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="31">
         <v>4</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>43</v>
-      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
-      <c r="J20" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="40"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="24"/>
-      <c r="E21" s="39"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" ht="14.15" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>42</v>
-      </c>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="35"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
-      <c r="J22" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="40"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="39"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
-      <c r="J23" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="46.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>44</v>
-      </c>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.45">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="J24" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
@@ -1489,16 +1446,6 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>